<commit_message>
master: ok coba2 tmaahin waktu, storage, dll
</commit_message>
<xml_diff>
--- a/opfga_step_by_step/system_data_costumize.xlsx
+++ b/opfga_step_by_step/system_data_costumize.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6200" activeTab="2"/>
+    <workbookView windowWidth="19200" windowHeight="6200"/>
   </bookViews>
   <sheets>
     <sheet name="bus_data" sheetId="1" r:id="rId1"/>
     <sheet name="gen_bus_map" sheetId="2" r:id="rId2"/>
-    <sheet name="cost_data" sheetId="3" r:id="rId3"/>
+    <sheet name="gen_thermal" sheetId="3" r:id="rId3"/>
     <sheet name="linedata" sheetId="4" r:id="rId4"/>
+    <sheet name="gen_hidro" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>bus</t>
   </si>
@@ -71,6 +72,24 @@
     <t>is_H2</t>
   </si>
   <si>
+    <t>Pmin</t>
+  </si>
+  <si>
+    <t>Pmax</t>
+  </si>
+  <si>
+    <t>Qmin</t>
+  </si>
+  <si>
+    <t>Qmax</t>
+  </si>
+  <si>
+    <t>Ramp_up</t>
+  </si>
+  <si>
+    <t>Ramp_down</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
@@ -80,16 +99,25 @@
     <t>c</t>
   </si>
   <si>
-    <t>Pmin</t>
-  </si>
-  <si>
-    <t>Pmax</t>
-  </si>
-  <si>
-    <t>Qmin</t>
-  </si>
-  <si>
-    <t>Qmax</t>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>B_half</t>
+  </si>
+  <si>
+    <t>Tap</t>
+  </si>
+  <si>
+    <t>Smax</t>
   </si>
   <si>
     <t>kH2</t>
@@ -98,28 +126,13 @@
     <t>priceH2</t>
   </si>
   <si>
+    <t>H2_cap</t>
+  </si>
+  <si>
+    <t>H2_init</t>
+  </si>
+  <si>
     <t>0.05</t>
-  </si>
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>B_half</t>
-  </si>
-  <si>
-    <t>Tap</t>
-  </si>
-  <si>
-    <t>Smax</t>
   </si>
 </sst>
 </file>
@@ -132,7 +145,7 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,13 +162,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -625,148 +631,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1126,8 +1132,8 @@
   <sheetPr/>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="6"/>
@@ -1233,15 +1239,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
+  <cols>
+    <col min="9" max="9" width="12.3636363636364" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1251,8 +1260,26 @@
       <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1262,8 +1289,26 @@
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>-50</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1272,6 +1317,24 @@
       </c>
       <c r="C3">
         <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>-50</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1283,47 +1346,29 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1335,56 +1380,6 @@
       </c>
       <c r="D2">
         <v>5</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>-50</v>
-      </c>
-      <c r="H2">
-        <v>50</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0.005</v>
-      </c>
-      <c r="F3">
-        <v>30</v>
-      </c>
-      <c r="G3">
-        <v>-50</v>
-      </c>
-      <c r="H3">
-        <v>50</v>
-      </c>
-      <c r="I3">
-        <v>60</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1399,32 +1394,32 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="6"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1494,6 +1489,57 @@
       </c>
       <c r="G4">
         <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>